<commit_message>
update order format extractor
</commit_message>
<xml_diff>
--- a/front/src/assets/template3.xlsx
+++ b/front/src/assets/template3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmy/Desktop/Betagouv/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E865137-6F97-994D-84B1-E74509DD3FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586B6342-907A-BD47-8300-F3BAF4ECCC6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="24580" windowHeight="14560" activeTab="2" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="24580" windowHeight="14560" activeTab="1" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
   <sheets>
     <sheet name="ETPT A-JUST" sheetId="1" r:id="rId1"/>
@@ -955,7 +955,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1030,9 +1030,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1539,7 +1536,7 @@
   <dimension ref="A1:DN8"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1571,131 +1568,131 @@
       </c>
     </row>
     <row r="2" spans="1:118" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="54"/>
-      <c r="Z2" s="54"/>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="54"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="54"/>
-      <c r="AF2" s="54"/>
-      <c r="AG2" s="54"/>
-      <c r="AH2" s="54"/>
-      <c r="AI2" s="54"/>
-      <c r="AJ2" s="54"/>
-      <c r="AK2" s="54"/>
-      <c r="AL2" s="54"/>
-      <c r="AM2" s="54"/>
-      <c r="AN2" s="54"/>
-      <c r="AO2" s="54"/>
-      <c r="AP2" s="54"/>
-      <c r="AQ2" s="54"/>
-      <c r="AR2" s="54"/>
-      <c r="AS2" s="54"/>
-      <c r="AT2" s="54"/>
-      <c r="AU2" s="54"/>
-      <c r="AV2" s="54"/>
-      <c r="AW2" s="54"/>
-      <c r="AX2" s="54"/>
-      <c r="AY2" s="54"/>
-      <c r="AZ2" s="54"/>
-      <c r="BA2" s="54"/>
-      <c r="BB2" s="54"/>
-      <c r="BC2" s="54"/>
-      <c r="BD2" s="54"/>
-      <c r="BE2" s="54"/>
-      <c r="BF2" s="54"/>
-      <c r="BG2" s="54"/>
-      <c r="BH2" s="54"/>
-      <c r="BI2" s="54"/>
-      <c r="BJ2" s="54"/>
-      <c r="BK2" s="54"/>
-      <c r="BL2" s="54"/>
-      <c r="BM2" s="54"/>
-      <c r="BN2" s="54"/>
-      <c r="BO2" s="54"/>
-      <c r="BP2" s="54"/>
-      <c r="BQ2" s="54"/>
-      <c r="BR2" s="54"/>
-      <c r="BS2" s="54"/>
-      <c r="BT2" s="54"/>
-      <c r="BU2" s="54"/>
-      <c r="BV2" s="54"/>
-      <c r="BW2" s="54"/>
-      <c r="BX2" s="54"/>
-      <c r="BY2" s="54"/>
-      <c r="BZ2" s="54"/>
-      <c r="CA2" s="54"/>
-      <c r="CB2" s="54"/>
-      <c r="CC2" s="54"/>
-      <c r="CD2" s="54"/>
-      <c r="CE2" s="54"/>
-      <c r="CF2" s="54"/>
-      <c r="CG2" s="54"/>
-      <c r="CH2" s="54"/>
-      <c r="CI2" s="54"/>
-      <c r="CJ2" s="54"/>
-      <c r="CK2" s="54"/>
-      <c r="CL2" s="54"/>
-      <c r="CM2" s="54"/>
-      <c r="CN2" s="54"/>
-      <c r="CO2" s="54"/>
-      <c r="CP2" s="54"/>
-      <c r="CQ2" s="54"/>
-      <c r="CR2" s="54"/>
-      <c r="CS2" s="54"/>
-      <c r="CT2" s="54"/>
-      <c r="CU2" s="54"/>
-      <c r="CV2" s="54"/>
-      <c r="CW2" s="54"/>
-      <c r="CX2" s="54"/>
-      <c r="CY2" s="54"/>
-      <c r="CZ2" s="54"/>
-      <c r="DA2" s="54"/>
-      <c r="DB2" s="54"/>
-      <c r="DC2" s="54"/>
-      <c r="DD2" s="54"/>
-      <c r="DE2" s="54"/>
-      <c r="DF2" s="54"/>
-      <c r="DG2" s="54"/>
-      <c r="DH2" s="54"/>
-      <c r="DI2" s="54"/>
-      <c r="DJ2" s="54"/>
-      <c r="DK2" s="54"/>
-      <c r="DL2" s="54"/>
-      <c r="DM2" s="54"/>
-      <c r="DN2" s="54"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="53"/>
+      <c r="Y2" s="53"/>
+      <c r="Z2" s="53"/>
+      <c r="AA2" s="53"/>
+      <c r="AB2" s="53"/>
+      <c r="AC2" s="53"/>
+      <c r="AD2" s="53"/>
+      <c r="AE2" s="53"/>
+      <c r="AF2" s="53"/>
+      <c r="AG2" s="53"/>
+      <c r="AH2" s="53"/>
+      <c r="AI2" s="53"/>
+      <c r="AJ2" s="53"/>
+      <c r="AK2" s="53"/>
+      <c r="AL2" s="53"/>
+      <c r="AM2" s="53"/>
+      <c r="AN2" s="53"/>
+      <c r="AO2" s="53"/>
+      <c r="AP2" s="53"/>
+      <c r="AQ2" s="53"/>
+      <c r="AR2" s="53"/>
+      <c r="AS2" s="53"/>
+      <c r="AT2" s="53"/>
+      <c r="AU2" s="53"/>
+      <c r="AV2" s="53"/>
+      <c r="AW2" s="53"/>
+      <c r="AX2" s="53"/>
+      <c r="AY2" s="53"/>
+      <c r="AZ2" s="53"/>
+      <c r="BA2" s="53"/>
+      <c r="BB2" s="53"/>
+      <c r="BC2" s="53"/>
+      <c r="BD2" s="53"/>
+      <c r="BE2" s="53"/>
+      <c r="BF2" s="53"/>
+      <c r="BG2" s="53"/>
+      <c r="BH2" s="53"/>
+      <c r="BI2" s="53"/>
+      <c r="BJ2" s="53"/>
+      <c r="BK2" s="53"/>
+      <c r="BL2" s="53"/>
+      <c r="BM2" s="53"/>
+      <c r="BN2" s="53"/>
+      <c r="BO2" s="53"/>
+      <c r="BP2" s="53"/>
+      <c r="BQ2" s="53"/>
+      <c r="BR2" s="53"/>
+      <c r="BS2" s="53"/>
+      <c r="BT2" s="53"/>
+      <c r="BU2" s="53"/>
+      <c r="BV2" s="53"/>
+      <c r="BW2" s="53"/>
+      <c r="BX2" s="53"/>
+      <c r="BY2" s="53"/>
+      <c r="BZ2" s="53"/>
+      <c r="CA2" s="53"/>
+      <c r="CB2" s="53"/>
+      <c r="CC2" s="53"/>
+      <c r="CD2" s="53"/>
+      <c r="CE2" s="53"/>
+      <c r="CF2" s="53"/>
+      <c r="CG2" s="53"/>
+      <c r="CH2" s="53"/>
+      <c r="CI2" s="53"/>
+      <c r="CJ2" s="53"/>
+      <c r="CK2" s="53"/>
+      <c r="CL2" s="53"/>
+      <c r="CM2" s="53"/>
+      <c r="CN2" s="53"/>
+      <c r="CO2" s="53"/>
+      <c r="CP2" s="53"/>
+      <c r="CQ2" s="53"/>
+      <c r="CR2" s="53"/>
+      <c r="CS2" s="53"/>
+      <c r="CT2" s="53"/>
+      <c r="CU2" s="53"/>
+      <c r="CV2" s="53"/>
+      <c r="CW2" s="53"/>
+      <c r="CX2" s="53"/>
+      <c r="CY2" s="53"/>
+      <c r="CZ2" s="53"/>
+      <c r="DA2" s="53"/>
+      <c r="DB2" s="53"/>
+      <c r="DC2" s="53"/>
+      <c r="DD2" s="53"/>
+      <c r="DE2" s="53"/>
+      <c r="DF2" s="53"/>
+      <c r="DG2" s="53"/>
+      <c r="DH2" s="53"/>
+      <c r="DI2" s="53"/>
+      <c r="DJ2" s="53"/>
+      <c r="DK2" s="53"/>
+      <c r="DL2" s="53"/>
+      <c r="DM2" s="53"/>
+      <c r="DN2" s="53"/>
     </row>
     <row r="3" spans="1:118" x14ac:dyDescent="0.2">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="57" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
@@ -1704,119 +1701,119 @@
       <c r="C3"/>
       <c r="D3"/>
       <c r="E3"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="56"/>
-      <c r="P3" s="56"/>
-      <c r="Q3" s="56"/>
-      <c r="R3" s="56"/>
-      <c r="S3" s="56"/>
-      <c r="T3" s="56"/>
-      <c r="U3" s="56"/>
-      <c r="V3" s="56"/>
-      <c r="W3" s="56"/>
-      <c r="X3" s="56"/>
-      <c r="Y3" s="56"/>
-      <c r="Z3" s="56"/>
-      <c r="AA3" s="56"/>
-      <c r="AB3" s="56"/>
-      <c r="AC3" s="56"/>
-      <c r="AD3" s="56"/>
-      <c r="AE3" s="56"/>
-      <c r="AF3" s="56"/>
-      <c r="AG3" s="56"/>
-      <c r="AH3" s="56"/>
-      <c r="AI3" s="56"/>
-      <c r="AJ3" s="56"/>
-      <c r="AK3" s="56"/>
-      <c r="AL3" s="56"/>
-      <c r="AM3" s="56"/>
-      <c r="AN3" s="56"/>
-      <c r="AO3" s="56"/>
-      <c r="AP3" s="56"/>
-      <c r="AQ3" s="56"/>
-      <c r="AR3" s="56"/>
-      <c r="AS3" s="56"/>
-      <c r="AT3" s="56"/>
-      <c r="AU3" s="56"/>
-      <c r="AV3" s="56"/>
-      <c r="AW3" s="56"/>
-      <c r="AX3" s="56"/>
-      <c r="AY3" s="56"/>
-      <c r="AZ3" s="56"/>
-      <c r="BA3" s="56"/>
-      <c r="BB3" s="56"/>
-      <c r="BC3" s="56"/>
-      <c r="BD3" s="56"/>
-      <c r="BE3" s="56"/>
-      <c r="BF3" s="56"/>
-      <c r="BG3" s="56"/>
-      <c r="BH3" s="56"/>
-      <c r="BI3" s="56"/>
-      <c r="BJ3" s="56"/>
-      <c r="BK3" s="56"/>
-      <c r="BL3" s="56"/>
-      <c r="BM3" s="56"/>
-      <c r="BN3" s="56"/>
-      <c r="BO3" s="56"/>
-      <c r="BP3" s="56"/>
-      <c r="BQ3" s="56"/>
-      <c r="BR3" s="56"/>
-      <c r="BS3" s="56"/>
-      <c r="BT3" s="56"/>
-      <c r="BU3" s="56"/>
-      <c r="BV3" s="56"/>
-      <c r="BW3" s="56"/>
-      <c r="BX3" s="56"/>
-      <c r="BY3" s="56"/>
-      <c r="BZ3" s="56"/>
-      <c r="CA3" s="56"/>
-      <c r="CB3" s="56"/>
-      <c r="CC3" s="56"/>
-      <c r="CD3" s="56"/>
-      <c r="CE3" s="56"/>
-      <c r="CF3" s="56"/>
-      <c r="CG3" s="56"/>
-      <c r="CH3" s="56"/>
-      <c r="CI3" s="56"/>
-      <c r="CJ3" s="56"/>
-      <c r="CK3" s="56"/>
-      <c r="CL3" s="56"/>
-      <c r="CM3" s="56"/>
-      <c r="CN3" s="56"/>
-      <c r="CO3" s="56"/>
-      <c r="CP3" s="56"/>
-      <c r="CQ3" s="56"/>
-      <c r="CR3" s="56"/>
-      <c r="CS3" s="56"/>
-      <c r="CT3" s="56"/>
-      <c r="CU3" s="56"/>
-      <c r="CV3" s="56"/>
-      <c r="CW3" s="56"/>
-      <c r="CX3" s="56"/>
-      <c r="CY3" s="56"/>
-      <c r="CZ3" s="56"/>
-      <c r="DA3" s="56"/>
-      <c r="DB3" s="56"/>
-      <c r="DC3" s="56"/>
-      <c r="DD3" s="56"/>
-      <c r="DE3" s="56"/>
-      <c r="DF3" s="56"/>
-      <c r="DG3" s="56"/>
-      <c r="DH3" s="56"/>
-      <c r="DI3" s="56"/>
-      <c r="DJ3" s="56"/>
-      <c r="DK3" s="56"/>
-      <c r="DL3" s="56"/>
-      <c r="DM3" s="56"/>
-      <c r="DN3" s="56"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="55"/>
+      <c r="R3" s="55"/>
+      <c r="S3" s="55"/>
+      <c r="T3" s="55"/>
+      <c r="U3" s="55"/>
+      <c r="V3" s="55"/>
+      <c r="W3" s="55"/>
+      <c r="X3" s="55"/>
+      <c r="Y3" s="55"/>
+      <c r="Z3" s="55"/>
+      <c r="AA3" s="55"/>
+      <c r="AB3" s="55"/>
+      <c r="AC3" s="55"/>
+      <c r="AD3" s="55"/>
+      <c r="AE3" s="55"/>
+      <c r="AF3" s="55"/>
+      <c r="AG3" s="55"/>
+      <c r="AH3" s="55"/>
+      <c r="AI3" s="55"/>
+      <c r="AJ3" s="55"/>
+      <c r="AK3" s="55"/>
+      <c r="AL3" s="55"/>
+      <c r="AM3" s="55"/>
+      <c r="AN3" s="55"/>
+      <c r="AO3" s="55"/>
+      <c r="AP3" s="55"/>
+      <c r="AQ3" s="55"/>
+      <c r="AR3" s="55"/>
+      <c r="AS3" s="55"/>
+      <c r="AT3" s="55"/>
+      <c r="AU3" s="55"/>
+      <c r="AV3" s="55"/>
+      <c r="AW3" s="55"/>
+      <c r="AX3" s="55"/>
+      <c r="AY3" s="55"/>
+      <c r="AZ3" s="55"/>
+      <c r="BA3" s="55"/>
+      <c r="BB3" s="55"/>
+      <c r="BC3" s="55"/>
+      <c r="BD3" s="55"/>
+      <c r="BE3" s="55"/>
+      <c r="BF3" s="55"/>
+      <c r="BG3" s="55"/>
+      <c r="BH3" s="55"/>
+      <c r="BI3" s="55"/>
+      <c r="BJ3" s="55"/>
+      <c r="BK3" s="55"/>
+      <c r="BL3" s="55"/>
+      <c r="BM3" s="55"/>
+      <c r="BN3" s="55"/>
+      <c r="BO3" s="55"/>
+      <c r="BP3" s="55"/>
+      <c r="BQ3" s="55"/>
+      <c r="BR3" s="55"/>
+      <c r="BS3" s="55"/>
+      <c r="BT3" s="55"/>
+      <c r="BU3" s="55"/>
+      <c r="BV3" s="55"/>
+      <c r="BW3" s="55"/>
+      <c r="BX3" s="55"/>
+      <c r="BY3" s="55"/>
+      <c r="BZ3" s="55"/>
+      <c r="CA3" s="55"/>
+      <c r="CB3" s="55"/>
+      <c r="CC3" s="55"/>
+      <c r="CD3" s="55"/>
+      <c r="CE3" s="55"/>
+      <c r="CF3" s="55"/>
+      <c r="CG3" s="55"/>
+      <c r="CH3" s="55"/>
+      <c r="CI3" s="55"/>
+      <c r="CJ3" s="55"/>
+      <c r="CK3" s="55"/>
+      <c r="CL3" s="55"/>
+      <c r="CM3" s="55"/>
+      <c r="CN3" s="55"/>
+      <c r="CO3" s="55"/>
+      <c r="CP3" s="55"/>
+      <c r="CQ3" s="55"/>
+      <c r="CR3" s="55"/>
+      <c r="CS3" s="55"/>
+      <c r="CT3" s="55"/>
+      <c r="CU3" s="55"/>
+      <c r="CV3" s="55"/>
+      <c r="CW3" s="55"/>
+      <c r="CX3" s="55"/>
+      <c r="CY3" s="55"/>
+      <c r="CZ3" s="55"/>
+      <c r="DA3" s="55"/>
+      <c r="DB3" s="55"/>
+      <c r="DC3" s="55"/>
+      <c r="DD3" s="55"/>
+      <c r="DE3" s="55"/>
+      <c r="DF3" s="55"/>
+      <c r="DG3" s="55"/>
+      <c r="DH3" s="55"/>
+      <c r="DI3" s="55"/>
+      <c r="DJ3" s="55"/>
+      <c r="DK3" s="55"/>
+      <c r="DL3" s="55"/>
+      <c r="DM3" s="55"/>
+      <c r="DN3" s="55"/>
     </row>
     <row r="4" spans="1:118" x14ac:dyDescent="0.2">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="57" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1849,11 +1846,6 @@
   </sheetData>
   <autoFilter ref="A2:DN2" xr:uid="{F3674A8A-13E9-4EDB-B294-D1FF8F18362C}"/>
   <dataConsolidate/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I1048576" xr:uid="{35CBB097-B87A-D144-AF9A-C29F979208B1}">
-      <formula1>#REF!</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1864,8 +1856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B89445B-6ECC-4440-B85C-E593AE209933}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1891,7 +1883,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="54" t="s">
         <v>66</v>
       </c>
       <c r="B2" t="s">
@@ -1899,7 +1891,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="57" t="s">
         <v>71</v>
       </c>
       <c r="B3" t="s">
@@ -1907,7 +1899,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="57" t="s">
         <v>71</v>
       </c>
       <c r="B4" t="s">
@@ -1930,7 +1922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E893F90-1EC7-764C-B747-7920FCEC73CB}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1949,10 +1941,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="45" t="s">
         <v>81</v>
       </c>
       <c r="C1" t="s">
@@ -1960,10 +1952,10 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="47" t="e">
+      <c r="B2" s="46" t="e">
         <f>VLOOKUP(A2,'codage tribunal'!A:B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
@@ -1975,31 +1967,31 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="39"/>
+      <c r="C3" s="38"/>
     </row>
     <row r="4" spans="1:13" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="42" t="s">
+      <c r="A4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="43" t="s">
+      <c r="H4" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="I4" s="43" t="s">
+      <c r="I4" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="J4" s="43" t="s">
+      <c r="J4" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="K4" s="44" t="s">
+      <c r="K4" s="43" t="s">
         <v>80</v>
       </c>
       <c r="L4" t="s">
@@ -2007,38 +1999,38 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="45"/>
-      <c r="C5" s="49" t="s">
+      <c r="A5" s="44"/>
+      <c r="C5" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="52" t="e">
+      <c r="E5" s="51" t="e">
         <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"M-TIT",'ETPT Format DDG'!$C:$C,$A$2)</f>
         <v>#N/A</v>
       </c>
-      <c r="F5" s="50" t="e">
+      <c r="F5" s="49" t="e">
         <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"M-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$2)</f>
         <v>#N/A</v>
       </c>
-      <c r="G5" s="50" t="e">
+      <c r="G5" s="49" t="e">
         <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"M-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$2)</f>
         <v>#N/A</v>
       </c>
-      <c r="H5" s="50" t="e">
+      <c r="H5" s="49" t="e">
         <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"F-TIT",'ETPT Format DDG'!$C:$C,$A$2)</f>
         <v>#N/A</v>
       </c>
-      <c r="I5" s="50" t="e">
+      <c r="I5" s="49" t="e">
         <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"F-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$2)</f>
         <v>#N/A</v>
       </c>
-      <c r="J5" s="50" t="e">
+      <c r="J5" s="49" t="e">
         <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"F-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$2)</f>
         <v>#N/A</v>
       </c>
-      <c r="K5" s="51" t="e">
+      <c r="K5" s="50" t="e">
         <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$DU,,IFERROR(MATCH(D5,'ETPT Format DDG'!$2:$2,0),MATCH(C5,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"C",'ETPT Format DDG'!$C:$C,$A$2)</f>
         <v>#N/A</v>
       </c>

</xml_diff>